<commit_message>
BC hoa hong hoadon - chi tiet: add colum {TenNVPhuTrach}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon_ChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon_ChiTiet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Tổng cộng:</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Thực tính</t>
+  </si>
+  <si>
+    <t>NV phụ trách</t>
   </si>
 </sst>
 </file>
@@ -333,29 +336,29 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -646,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,631 +660,659 @@
     <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
     <col min="2" max="3" width="20.28515625" style="10" customWidth="1"/>
     <col min="4" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="34" style="20" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="15" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="15" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13" style="3" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="26" style="3" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="7" width="20.42578125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="34" style="20" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" style="15" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13" style="3" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="26" style="3" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="F2" s="26"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-    </row>
-    <row r="3" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="26"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+    </row>
+    <row r="3" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="F3" s="26"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="29"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="29"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="26"/>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
-    </row>
-    <row r="4" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="R3" s="29"/>
+    </row>
+    <row r="4" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="J4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="K4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="L4" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="35"/>
+      <c r="N4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="O4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32" t="s">
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="32" t="s">
+      <c r="R4" s="35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="24" t="s">
+    <row r="5" spans="1:19" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="M5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="31"/>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="37"/>
+      <c r="O5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="P5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="19"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="21"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="23"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="5"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="19"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="21"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="5"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="21"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="5"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="5"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="13"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="19"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="5"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="19"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="5"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="5"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="19"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="13"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="19"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="5"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="5"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="5"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="21"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="5"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="5"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="5"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="5"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="13"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="5"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="13"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="5"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="5"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="21"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="5"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="13"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="5"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="19"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="5"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="5"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="5"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="5"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="5"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="13"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="5"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="13"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="5"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="13"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="1:18" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="16"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
       <c r="J30" s="16"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="6">
-        <f>SUM(L$6:L29)</f>
+      <c r="K30" s="16"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="6">
+        <f>SUM(M$6:M29)</f>
         <v>0</v>
       </c>
-      <c r="M30" s="6"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="6">
-        <f>SUM(O$6:O29)</f>
-        <v>0</v>
-      </c>
+      <c r="O30" s="6"/>
       <c r="P30" s="6">
         <f>SUM(P$6:P29)</f>
         <v>0</v>
@@ -1290,27 +1321,32 @@
         <f>SUM(Q$6:Q29)</f>
         <v>0</v>
       </c>
+      <c r="R30" s="6">
+        <f>SUM(R$6:R29)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="G2:Q2"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A1:Q1"/>
+  <mergeCells count="19">
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H2:R2"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A1:R1"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="R4:R5"/>
     <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="P4:P5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
- BC hoahong hoadon-chitiet: add {MaNVPhuTrach}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon_ChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon_ChiTiet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Tổng cộng:</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>NV phụ trách</t>
+  </si>
+  <si>
+    <t>Mã NV phụ trách</t>
   </si>
 </sst>
 </file>
@@ -336,6 +339,15 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -350,15 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -649,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,159 +663,166 @@
     <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
     <col min="2" max="3" width="20.28515625" style="10" customWidth="1"/>
     <col min="4" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="20.42578125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="34" style="20" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" style="15" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13" style="3" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="26" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="8" width="20.42578125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="34" style="20" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="15" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" style="15" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="13" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="26" style="3" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-    </row>
-    <row r="3" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="26"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+    </row>
+    <row r="3" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="29"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="29"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="26"/>
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
       <c r="R3" s="29"/>
-    </row>
-    <row r="4" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="S3" s="29"/>
+    </row>
+    <row r="4" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="I4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="J4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="K4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="L4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="M4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="36" t="s">
+      <c r="N4" s="32"/>
+      <c r="O4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="P4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35" t="s">
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="35" t="s">
+      <c r="S4" s="32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="24" t="s">
+    <row r="5" spans="1:20" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="N5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="37"/>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="31"/>
+      <c r="P5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="Q5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -820,19 +830,20 @@
       <c r="E6" s="9"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="5"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="23"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -840,19 +851,20 @@
       <c r="E7" s="9"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="5"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -860,19 +872,20 @@
       <c r="E8" s="9"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="5"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="21"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="13"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -880,19 +893,20 @@
       <c r="E9" s="9"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="5"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="21"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -900,19 +914,20 @@
       <c r="E10" s="9"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="5"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -920,19 +935,20 @@
       <c r="E11" s="9"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="5"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -940,19 +956,20 @@
       <c r="E12" s="9"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="5"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -960,19 +977,20 @@
       <c r="E13" s="9"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="5"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="13"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -980,19 +998,20 @@
       <c r="E14" s="9"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="5"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="13"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1000,19 +1019,20 @@
       <c r="E15" s="9"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="5"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="13"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1020,19 +1040,20 @@
       <c r="E16" s="9"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="5"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="13"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1040,19 +1061,20 @@
       <c r="E17" s="9"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="5"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="13"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1060,19 +1082,20 @@
       <c r="E18" s="9"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="5"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="13"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1080,19 +1103,20 @@
       <c r="E19" s="9"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="5"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="13"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1100,19 +1124,20 @@
       <c r="E20" s="9"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="5"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="13"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1120,19 +1145,20 @@
       <c r="E21" s="9"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="5"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1140,19 +1166,20 @@
       <c r="E22" s="9"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="5"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="21"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="13"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -1160,19 +1187,20 @@
       <c r="E23" s="9"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="5"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="13"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1180,19 +1208,20 @@
       <c r="E24" s="9"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="5"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="21"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="13"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="5"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1200,19 +1229,20 @@
       <c r="E25" s="9"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="5"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="21"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="13"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="5"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -1220,19 +1250,20 @@
       <c r="E26" s="9"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="5"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="21"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="13"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1240,19 +1271,20 @@
       <c r="E27" s="9"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="5"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="13"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1260,19 +1292,20 @@
       <c r="E28" s="9"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="5"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="21"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="13"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -1280,43 +1313,41 @@
       <c r="E29" s="9"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="5"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="13"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
-    </row>
-    <row r="30" spans="1:18" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+      <c r="S29" s="5"/>
+    </row>
+    <row r="30" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="16"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="6">
-        <f>SUM(M$6:M29)</f>
+      <c r="L30" s="16"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="6">
+        <f>SUM(N$6:N29)</f>
         <v>0</v>
       </c>
-      <c r="N30" s="6"/>
       <c r="O30" s="6"/>
-      <c r="P30" s="6">
-        <f>SUM(P$6:P29)</f>
-        <v>0</v>
-      </c>
+      <c r="P30" s="6"/>
       <c r="Q30" s="6">
         <f>SUM(Q$6:Q29)</f>
         <v>0</v>
@@ -1325,28 +1356,33 @@
         <f>SUM(R$6:R29)</f>
         <v>0</v>
       </c>
+      <c r="S30" s="6">
+        <f>SUM(S$6:S29)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H2:R2"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A1:R1"/>
+  <mergeCells count="20">
+    <mergeCell ref="A1:S1"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="S4:S5"/>
     <mergeCell ref="R4:R5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I2:S2"/>
+    <mergeCell ref="A30:J30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
check lại phần xuất excel
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon_ChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongHoaDon_ChiTiet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">BÁO CÁO TỔNG HỢP HOA HỒNG CHI TIẾT THEO HÓA ĐƠN </t>
   </si>
@@ -80,10 +80,16 @@
     <t>Thực tính</t>
   </si>
   <si>
-    <t>NV phụ trách</t>
-  </si>
-  <si>
-    <t>Mã NV phụ trách</t>
+    <t>Mã TV chính</t>
+  </si>
+  <si>
+    <t>Tên TV chính</t>
+  </si>
+  <si>
+    <t>Mã TV phụ</t>
+  </si>
+  <si>
+    <t>Tên TV phụ</t>
   </si>
 </sst>
 </file>
@@ -283,6 +289,9 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -292,14 +301,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J4" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,22 +607,22 @@
     <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
     <col min="2" max="3" width="20.28515625" style="8" customWidth="1"/>
     <col min="4" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="8" width="20.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="34" style="16" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" style="12" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="22.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="26" style="3" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="10" width="20.42578125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="34" style="16" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" style="12" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="13" style="3" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="26" style="3" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -629,138 +635,152 @@
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-    </row>
-    <row r="3" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+    </row>
+    <row r="3" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
-      <c r="I3" s="21"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="22"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="25"/>
       <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
+      <c r="O3" s="22"/>
       <c r="P3" s="25"/>
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
-    </row>
-    <row r="4" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+    </row>
+    <row r="4" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="L4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="M4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="N4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="O4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27" t="s">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="R4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26" t="s">
+      <c r="S4" s="27"/>
+      <c r="T4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="26" t="s">
+      <c r="U4" s="27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="20" t="s">
+    <row r="5" spans="1:22" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="P5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="20" t="s">
+      <c r="Q5" s="29"/>
+      <c r="R5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="S5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -769,19 +789,21 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="19"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="O6" s="19"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -790,19 +812,21 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="11"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="O7" s="11"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -811,19 +835,21 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="11"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="O8" s="11"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -832,19 +858,21 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="11"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="O9" s="11"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -853,19 +881,21 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="11"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="O10" s="11"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -874,19 +904,21 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="11"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="O11" s="11"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -895,19 +927,21 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="11"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="O12" s="11"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -916,19 +950,21 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="11"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="O13" s="11"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -937,19 +973,21 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="11"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="O14" s="11"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -958,19 +996,21 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="11"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="O15" s="11"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -979,19 +1019,21 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="11"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="O16" s="11"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1000,19 +1042,21 @@
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="11"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
+      <c r="O17" s="11"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1021,19 +1065,21 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="11"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+      <c r="O18" s="11"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1042,19 +1088,21 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="11"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
+      <c r="O19" s="11"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1063,19 +1111,21 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="11"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="O20" s="11"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1084,19 +1134,21 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="11"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
+      <c r="O21" s="11"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1105,19 +1157,21 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="11"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
+      <c r="O22" s="11"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1126,19 +1180,21 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="11"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="O23" s="11"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1147,19 +1203,21 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="11"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
+      <c r="O24" s="11"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1168,19 +1226,21 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="11"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="O25" s="11"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1189,19 +1249,21 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="11"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1210,19 +1272,21 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="11"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="O27" s="11"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1231,19 +1295,21 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="11"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
+      <c r="O28" s="11"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1252,39 +1318,43 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="11"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
+      <c r="O29" s="11"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I2:S2"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K2:U2"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="T4:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>